<commit_message>
Updated A1 and A2
</commit_message>
<xml_diff>
--- a/yt_Dispatcher/Config.xlsx
+++ b/yt_Dispatcher/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\ドキュメント\UiPath\scr@pe.ai\yt_Dispatcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a3b1b6b23fc8a11/ドキュメント/UiPath/scr@pe.ai/yt_Dispatcher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54669664-B6B9-46DA-BE3D-A5D0F9013092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{54669664-B6B9-46DA-BE3D-A5D0F9013092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B86CC4D7-B05F-455A-884F-FDDD447A242B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>TargetChannel ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>QueueName</t>
   </si>
@@ -36,7 +33,16 @@
     <t>yt_queue</t>
   </si>
   <si>
-    <t>RealCharlieKirk</t>
+    <t>TargetChannelName</t>
+  </si>
+  <si>
+    <t>TargetChannelID</t>
+  </si>
+  <si>
+    <t>CharlieKirk</t>
+  </si>
+  <si>
+    <t>UCfaIu2jO-fppCQV_lchCRIQ</t>
   </si>
 </sst>
 </file>
@@ -380,32 +386,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Performer A3 - Sentiment Analysis : Done
</commit_message>
<xml_diff>
--- a/yt_Dispatcher/Config.xlsx
+++ b/yt_Dispatcher/Config.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a3b1b6b23fc8a11/ドキュメント/UiPath/scr@pe.ai/yt_Dispatcher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{54669664-B6B9-46DA-BE3D-A5D0F9013092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B86CC4D7-B05F-455A-884F-FDDD447A242B}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{54669664-B6B9-46DA-BE3D-A5D0F9013092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C3FDC2B-9123-41A1-A2F6-FFDA71800AAD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TargetChannelDetails" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>QueueName</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>UCfaIu2jO-fppCQV_lchCRIQ</t>
+  </si>
+  <si>
+    <t>UCsBjURrPoezykLs9EqgamOA</t>
+  </si>
+  <si>
+    <t>Fireship</t>
   </si>
 </sst>
 </file>
@@ -101,11 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,17 +393,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24" style="4" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -411,13 +419,24 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>